<commit_message>
conexion a la base de datos de karenderia y  sincronizacion de datos
</commit_message>
<xml_diff>
--- a/listaproductos.xlsx
+++ b/listaproductos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\chileno\Karenderia Multiple Restaurant System subir lista\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1ACDBD1-5BCA-4751-90B2-BFAFC5A2CBA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E068D1-5BBD-44AB-8DEF-2EF394275500}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="466">
   <si>
     <t>SKU</t>
   </si>
@@ -1417,6 +1417,12 @@
   </si>
   <si>
     <t>83064c2b-f39b-467d-add6-2b220c55e0e3.jpg</t>
+  </si>
+  <si>
+    <t>demo</t>
+  </si>
+  <si>
+    <t>producto demo</t>
   </si>
 </sst>
 </file>
@@ -1787,10 +1793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F298"/>
+  <dimension ref="A1:F299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="C289" workbookViewId="0">
+      <selection activeCell="C302" sqref="C302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7749,6 +7755,23 @@
         <v>25990</v>
       </c>
       <c r="F298" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299" s="2">
+        <v>0</v>
+      </c>
+      <c r="B299" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="C299" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="E299" s="2">
+        <v>10</v>
+      </c>
+      <c r="F299" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
formato del excel actualizado
</commit_message>
<xml_diff>
--- a/listaproductos.xlsx
+++ b/listaproductos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\chileno\Karenderia Multiple Restaurant System subir lista\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E068D1-5BBD-44AB-8DEF-2EF394275500}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C40D80-B4EF-4283-886C-9EBD8C5F19BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20265" yWindow="75" windowWidth="20610" windowHeight="10995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCTOS" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="467">
   <si>
     <t>SKU</t>
   </si>
@@ -1423,6 +1423,9 @@
   </si>
   <si>
     <t>producto demo</t>
+  </si>
+  <si>
+    <t>logoproducto.jpeg</t>
   </si>
 </sst>
 </file>
@@ -1795,8 +1798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C289" workbookViewId="0">
-      <selection activeCell="C302" sqref="C302"/>
+    <sheetView tabSelected="1" topLeftCell="C248" workbookViewId="0">
+      <selection activeCell="F259" sqref="F259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,8 +1847,8 @@
       <c r="E2" s="2">
         <v>990</v>
       </c>
-      <c r="F2" s="3">
-        <v>0</v>
+      <c r="F2" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1864,8 +1867,8 @@
       <c r="E3" s="2">
         <v>990</v>
       </c>
-      <c r="F3" s="3">
-        <v>0</v>
+      <c r="F3" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1944,8 +1947,8 @@
       <c r="E7" s="2">
         <v>990</v>
       </c>
-      <c r="F7" s="3">
-        <v>0</v>
+      <c r="F7" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1964,8 +1967,8 @@
       <c r="E8" s="2">
         <v>990</v>
       </c>
-      <c r="F8" s="3">
-        <v>0</v>
+      <c r="F8" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2064,8 +2067,8 @@
       <c r="E13" s="2">
         <v>1250</v>
       </c>
-      <c r="F13" s="3">
-        <v>0</v>
+      <c r="F13" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2084,8 +2087,8 @@
       <c r="E14" s="2">
         <v>1250</v>
       </c>
-      <c r="F14" s="3">
-        <v>0</v>
+      <c r="F14" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2144,8 +2147,8 @@
       <c r="E17" s="2">
         <v>1250</v>
       </c>
-      <c r="F17" s="3">
-        <v>0</v>
+      <c r="F17" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2344,8 +2347,8 @@
       <c r="E27" s="2">
         <v>2100</v>
       </c>
-      <c r="F27" s="3">
-        <v>0</v>
+      <c r="F27" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2464,8 +2467,8 @@
       <c r="E33" s="2">
         <v>2100</v>
       </c>
-      <c r="F33" s="3">
-        <v>0</v>
+      <c r="F33" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2504,8 +2507,8 @@
       <c r="E35" s="2">
         <v>1490</v>
       </c>
-      <c r="F35" s="3">
-        <v>0</v>
+      <c r="F35" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2644,8 +2647,8 @@
       <c r="E42" s="2">
         <v>1490</v>
       </c>
-      <c r="F42" s="3">
-        <v>0</v>
+      <c r="F42" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2744,8 +2747,8 @@
       <c r="E47" s="2">
         <v>1800</v>
       </c>
-      <c r="F47" s="3">
-        <v>0</v>
+      <c r="F47" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2764,8 +2767,8 @@
       <c r="E48" s="2">
         <v>1800</v>
       </c>
-      <c r="F48" s="3">
-        <v>0</v>
+      <c r="F48" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2824,8 +2827,8 @@
       <c r="E51" s="2">
         <v>2100</v>
       </c>
-      <c r="F51" s="3">
-        <v>0</v>
+      <c r="F51" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2884,8 +2887,8 @@
       <c r="E54" s="2">
         <v>1700</v>
       </c>
-      <c r="F54" s="3">
-        <v>0</v>
+      <c r="F54" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2904,8 +2907,8 @@
       <c r="E55" s="2">
         <v>1700</v>
       </c>
-      <c r="F55" s="3">
-        <v>0</v>
+      <c r="F55" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2924,8 +2927,8 @@
       <c r="E56" s="2">
         <v>1700</v>
       </c>
-      <c r="F56" s="3">
-        <v>0</v>
+      <c r="F56" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2984,8 +2987,8 @@
       <c r="E59" s="2">
         <v>1700</v>
       </c>
-      <c r="F59" s="3">
-        <v>0</v>
+      <c r="F59" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -3004,8 +3007,8 @@
       <c r="E60" s="2">
         <v>1850</v>
       </c>
-      <c r="F60" s="3">
-        <v>0</v>
+      <c r="F60" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -3024,8 +3027,8 @@
       <c r="E61" s="2">
         <v>1700</v>
       </c>
-      <c r="F61" s="3">
-        <v>0</v>
+      <c r="F61" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -3044,8 +3047,8 @@
       <c r="E62" s="2">
         <v>1600</v>
       </c>
-      <c r="F62" s="3">
-        <v>0</v>
+      <c r="F62" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -3064,8 +3067,8 @@
       <c r="E63" s="2">
         <v>2650</v>
       </c>
-      <c r="F63" s="3">
-        <v>0</v>
+      <c r="F63" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -3084,8 +3087,8 @@
       <c r="E64" s="2">
         <v>1600</v>
       </c>
-      <c r="F64" s="3">
-        <v>0</v>
+      <c r="F64" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -3104,8 +3107,8 @@
       <c r="E65" s="2">
         <v>1600</v>
       </c>
-      <c r="F65" s="3">
-        <v>0</v>
+      <c r="F65" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -3124,8 +3127,8 @@
       <c r="E66" s="2">
         <v>1600</v>
       </c>
-      <c r="F66" s="3">
-        <v>0</v>
+      <c r="F66" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -3144,8 +3147,8 @@
       <c r="E67" s="2">
         <v>1700</v>
       </c>
-      <c r="F67" s="3">
-        <v>0</v>
+      <c r="F67" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -3164,8 +3167,8 @@
       <c r="E68" s="2">
         <v>1700</v>
       </c>
-      <c r="F68" s="3">
-        <v>0</v>
+      <c r="F68" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -3184,8 +3187,8 @@
       <c r="E69" s="2">
         <v>1700</v>
       </c>
-      <c r="F69" s="3">
-        <v>0</v>
+      <c r="F69" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -3204,8 +3207,8 @@
       <c r="E70" s="2">
         <v>1600</v>
       </c>
-      <c r="F70" s="3">
-        <v>0</v>
+      <c r="F70" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -3224,8 +3227,8 @@
       <c r="E71" s="2">
         <v>1700</v>
       </c>
-      <c r="F71" s="3">
-        <v>0</v>
+      <c r="F71" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -3244,8 +3247,8 @@
       <c r="E72" s="2">
         <v>1800</v>
       </c>
-      <c r="F72" s="3">
-        <v>0</v>
+      <c r="F72" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -3264,8 +3267,8 @@
       <c r="E73" s="2">
         <v>1700</v>
       </c>
-      <c r="F73" s="3">
-        <v>0</v>
+      <c r="F73" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -3284,8 +3287,8 @@
       <c r="E74" s="2">
         <v>1700</v>
       </c>
-      <c r="F74" s="3">
-        <v>0</v>
+      <c r="F74" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -3304,8 +3307,8 @@
       <c r="E75" s="2">
         <v>1700</v>
       </c>
-      <c r="F75" s="3">
-        <v>0</v>
+      <c r="F75" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -3344,8 +3347,8 @@
       <c r="E77" s="2">
         <v>5500</v>
       </c>
-      <c r="F77" s="3">
-        <v>0</v>
+      <c r="F77" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -3364,8 +3367,8 @@
       <c r="E78" s="2">
         <v>4990</v>
       </c>
-      <c r="F78" s="3">
-        <v>0</v>
+      <c r="F78" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -3384,8 +3387,8 @@
       <c r="E79" s="2">
         <v>4990</v>
       </c>
-      <c r="F79" s="3">
-        <v>0</v>
+      <c r="F79" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -3404,8 +3407,8 @@
       <c r="E80" s="2">
         <v>5500</v>
       </c>
-      <c r="F80" s="3">
-        <v>0</v>
+      <c r="F80" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -3444,8 +3447,8 @@
       <c r="E82" s="2">
         <v>3900</v>
       </c>
-      <c r="F82" s="3">
-        <v>0</v>
+      <c r="F82" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -3484,8 +3487,8 @@
       <c r="E84" s="2">
         <v>6190</v>
       </c>
-      <c r="F84" s="3">
-        <v>0</v>
+      <c r="F84" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -3524,8 +3527,8 @@
       <c r="E86" s="2">
         <v>4990</v>
       </c>
-      <c r="F86" s="3">
-        <v>0</v>
+      <c r="F86" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -3584,8 +3587,8 @@
       <c r="E89" s="2">
         <v>5800</v>
       </c>
-      <c r="F89" s="3">
-        <v>0</v>
+      <c r="F89" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -3644,8 +3647,8 @@
       <c r="E92" s="2">
         <v>4500</v>
       </c>
-      <c r="F92" s="3">
-        <v>0</v>
+      <c r="F92" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -3664,8 +3667,8 @@
       <c r="E93" s="2">
         <v>4990</v>
       </c>
-      <c r="F93" s="3">
-        <v>0</v>
+      <c r="F93" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3684,8 +3687,8 @@
       <c r="E94" s="2">
         <v>4600</v>
       </c>
-      <c r="F94" s="3">
-        <v>0</v>
+      <c r="F94" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -3704,8 +3707,8 @@
       <c r="E95" s="2">
         <v>6500</v>
       </c>
-      <c r="F95" s="3">
-        <v>0</v>
+      <c r="F95" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -3724,8 +3727,8 @@
       <c r="E96" s="2">
         <v>3000</v>
       </c>
-      <c r="F96" s="3">
-        <v>0</v>
+      <c r="F96" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3744,8 +3747,8 @@
       <c r="E97" s="2">
         <v>4200</v>
       </c>
-      <c r="F97" s="3">
-        <v>0</v>
+      <c r="F97" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3784,8 +3787,8 @@
       <c r="E99" s="2">
         <v>2990</v>
       </c>
-      <c r="F99" s="3">
-        <v>0</v>
+      <c r="F99" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3804,8 +3807,8 @@
       <c r="E100" s="2">
         <v>2990</v>
       </c>
-      <c r="F100" s="3">
-        <v>0</v>
+      <c r="F100" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -3824,8 +3827,8 @@
       <c r="E101" s="2">
         <v>3390</v>
       </c>
-      <c r="F101" s="3">
-        <v>0</v>
+      <c r="F101" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -3844,8 +3847,8 @@
       <c r="E102" s="2">
         <v>3390</v>
       </c>
-      <c r="F102" s="3">
-        <v>0</v>
+      <c r="F102" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -3904,8 +3907,8 @@
       <c r="E105" s="2">
         <v>3990</v>
       </c>
-      <c r="F105" s="3">
-        <v>0</v>
+      <c r="F105" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -3944,8 +3947,8 @@
       <c r="E107" s="2">
         <v>3590</v>
       </c>
-      <c r="F107" s="3">
-        <v>0</v>
+      <c r="F107" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -3984,8 +3987,8 @@
       <c r="E109" s="2">
         <v>3990</v>
       </c>
-      <c r="F109" s="3">
-        <v>0</v>
+      <c r="F109" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -4004,8 +4007,8 @@
       <c r="E110" s="2">
         <v>4690</v>
       </c>
-      <c r="F110" s="3">
-        <v>0</v>
+      <c r="F110" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -4024,8 +4027,8 @@
       <c r="E111" s="2">
         <v>4990</v>
       </c>
-      <c r="F111" s="3">
-        <v>0</v>
+      <c r="F111" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -4164,8 +4167,8 @@
       <c r="E118" s="2">
         <v>3400</v>
       </c>
-      <c r="F118" s="3">
-        <v>0</v>
+      <c r="F118" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -4204,8 +4207,8 @@
       <c r="E120" s="2">
         <v>2790</v>
       </c>
-      <c r="F120" s="3">
-        <v>0</v>
+      <c r="F120" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -4224,8 +4227,8 @@
       <c r="E121" s="2">
         <v>5990</v>
       </c>
-      <c r="F121" s="3">
-        <v>0</v>
+      <c r="F121" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -4284,8 +4287,8 @@
       <c r="E124" s="2">
         <v>4390</v>
       </c>
-      <c r="F124" s="3">
-        <v>0</v>
+      <c r="F124" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -4304,8 +4307,8 @@
       <c r="E125" s="2">
         <v>5990</v>
       </c>
-      <c r="F125" s="3">
-        <v>0</v>
+      <c r="F125" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -4384,8 +4387,8 @@
       <c r="E129" s="2">
         <v>4390</v>
       </c>
-      <c r="F129" s="3">
-        <v>0</v>
+      <c r="F129" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -4424,8 +4427,8 @@
       <c r="E131" s="2">
         <v>10990</v>
       </c>
-      <c r="F131" s="3">
-        <v>0</v>
+      <c r="F131" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -4444,8 +4447,8 @@
       <c r="E132" s="2">
         <v>10990</v>
       </c>
-      <c r="F132" s="3">
-        <v>0</v>
+      <c r="F132" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -4464,8 +4467,8 @@
       <c r="E133" s="2">
         <v>10990</v>
       </c>
-      <c r="F133" s="3">
-        <v>0</v>
+      <c r="F133" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -4484,8 +4487,8 @@
       <c r="E134" s="2">
         <v>10990</v>
       </c>
-      <c r="F134" s="3">
-        <v>0</v>
+      <c r="F134" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -4504,8 +4507,8 @@
       <c r="E135" s="2">
         <v>10990</v>
       </c>
-      <c r="F135" s="3">
-        <v>0</v>
+      <c r="F135" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -4604,8 +4607,8 @@
       <c r="E140" s="2">
         <v>4790</v>
       </c>
-      <c r="F140" s="3">
-        <v>0</v>
+      <c r="F140" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -4624,8 +4627,8 @@
       <c r="E141" s="2">
         <v>4790</v>
       </c>
-      <c r="F141" s="3">
-        <v>0</v>
+      <c r="F141" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -4664,8 +4667,8 @@
       <c r="E143" s="2">
         <v>3990</v>
       </c>
-      <c r="F143" s="3">
-        <v>0</v>
+      <c r="F143" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -4684,8 +4687,8 @@
       <c r="E144" s="2">
         <v>3990</v>
       </c>
-      <c r="F144" s="3">
-        <v>0</v>
+      <c r="F144" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -4704,8 +4707,8 @@
       <c r="E145" s="2">
         <v>4690</v>
       </c>
-      <c r="F145" s="3">
-        <v>0</v>
+      <c r="F145" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -4784,8 +4787,8 @@
       <c r="E149" s="2">
         <v>4990</v>
       </c>
-      <c r="F149" s="3">
-        <v>0</v>
+      <c r="F149" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -4804,8 +4807,8 @@
       <c r="E150" s="2">
         <v>11990</v>
       </c>
-      <c r="F150" s="3">
-        <v>0</v>
+      <c r="F150" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -4824,8 +4827,8 @@
       <c r="E151" s="2">
         <v>4290</v>
       </c>
-      <c r="F151" s="3">
-        <v>0</v>
+      <c r="F151" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -4844,8 +4847,8 @@
       <c r="E152" s="2">
         <v>3990</v>
       </c>
-      <c r="F152" s="3">
-        <v>0</v>
+      <c r="F152" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4864,8 +4867,8 @@
       <c r="E153" s="2">
         <v>11990</v>
       </c>
-      <c r="F153" s="3">
-        <v>0</v>
+      <c r="F153" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4884,8 +4887,8 @@
       <c r="E154" s="2">
         <v>4290</v>
       </c>
-      <c r="F154" s="3">
-        <v>0</v>
+      <c r="F154" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4904,8 +4907,8 @@
       <c r="E155" s="2">
         <v>13990</v>
       </c>
-      <c r="F155" s="3">
-        <v>0</v>
+      <c r="F155" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4924,8 +4927,8 @@
       <c r="E156" s="2">
         <v>4990</v>
       </c>
-      <c r="F156" s="3">
-        <v>0</v>
+      <c r="F156" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4960,8 +4963,8 @@
       <c r="E158" s="2">
         <v>2500</v>
       </c>
-      <c r="F158" s="3">
-        <v>0</v>
+      <c r="F158" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4998,8 +5001,8 @@
       <c r="E160" s="2">
         <v>5390</v>
       </c>
-      <c r="F160" s="3">
-        <v>0</v>
+      <c r="F160" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -5158,8 +5161,8 @@
       <c r="E168" s="2">
         <v>9990</v>
       </c>
-      <c r="F168" s="3">
-        <v>0</v>
+      <c r="F168" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -5178,8 +5181,8 @@
       <c r="E169" s="2">
         <v>5990</v>
       </c>
-      <c r="F169" s="3">
-        <v>0</v>
+      <c r="F169" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -5218,8 +5221,8 @@
       <c r="E171" s="2">
         <v>8290</v>
       </c>
-      <c r="F171" s="3">
-        <v>0</v>
+      <c r="F171" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -5238,8 +5241,8 @@
       <c r="E172" s="2">
         <v>8190</v>
       </c>
-      <c r="F172" s="3">
-        <v>0</v>
+      <c r="F172" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -5258,8 +5261,8 @@
       <c r="E173" s="2">
         <v>6890</v>
       </c>
-      <c r="F173" s="3">
-        <v>0</v>
+      <c r="F173" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -5278,8 +5281,8 @@
       <c r="E174" s="2">
         <v>5990</v>
       </c>
-      <c r="F174" s="3">
-        <v>0</v>
+      <c r="F174" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -5398,8 +5401,8 @@
       <c r="E180" s="2">
         <v>3990</v>
       </c>
-      <c r="F180" s="3">
-        <v>0</v>
+      <c r="F180" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -5418,8 +5421,8 @@
       <c r="E181" s="2">
         <v>19990</v>
       </c>
-      <c r="F181" s="3">
-        <v>0</v>
+      <c r="F181" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -5458,8 +5461,8 @@
       <c r="E183" s="2">
         <v>14990</v>
       </c>
-      <c r="F183" s="3">
-        <v>0</v>
+      <c r="F183" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
@@ -5478,8 +5481,8 @@
       <c r="E184" s="2">
         <v>18990</v>
       </c>
-      <c r="F184" s="3">
-        <v>0</v>
+      <c r="F184" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
@@ -5498,8 +5501,8 @@
       <c r="E185" s="2">
         <v>12990</v>
       </c>
-      <c r="F185" s="3">
-        <v>0</v>
+      <c r="F185" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
@@ -5518,8 +5521,8 @@
       <c r="E186" s="2">
         <v>15990</v>
       </c>
-      <c r="F186" s="3">
-        <v>0</v>
+      <c r="F186" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -5558,8 +5561,8 @@
       <c r="E188" s="2">
         <v>7990</v>
       </c>
-      <c r="F188" s="3">
-        <v>0</v>
+      <c r="F188" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
@@ -5578,8 +5581,8 @@
       <c r="E189" s="2">
         <v>5290</v>
       </c>
-      <c r="F189" s="3">
-        <v>0</v>
+      <c r="F189" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -5618,8 +5621,8 @@
       <c r="E191" s="2">
         <v>10990</v>
       </c>
-      <c r="F191" s="3">
-        <v>0</v>
+      <c r="F191" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
@@ -5638,8 +5641,8 @@
       <c r="E192" s="2">
         <v>9990</v>
       </c>
-      <c r="F192" s="3">
-        <v>0</v>
+      <c r="F192" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -5658,8 +5661,8 @@
       <c r="E193" s="2">
         <v>10990</v>
       </c>
-      <c r="F193" s="3">
-        <v>0</v>
+      <c r="F193" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
@@ -5698,8 +5701,8 @@
       <c r="E195" s="2">
         <v>9890</v>
       </c>
-      <c r="F195" s="3">
-        <v>0</v>
+      <c r="F195" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -5718,8 +5721,8 @@
       <c r="E196" s="2">
         <v>10990</v>
       </c>
-      <c r="F196" s="3">
-        <v>0</v>
+      <c r="F196" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
@@ -5738,8 +5741,8 @@
       <c r="E197" s="2">
         <v>6990</v>
       </c>
-      <c r="F197" s="3">
-        <v>0</v>
+      <c r="F197" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
@@ -5758,8 +5761,8 @@
       <c r="E198" s="2">
         <v>5590</v>
       </c>
-      <c r="F198" s="3">
-        <v>0</v>
+      <c r="F198" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
@@ -5778,8 +5781,8 @@
       <c r="E199" s="2">
         <v>3990</v>
       </c>
-      <c r="F199" s="3">
-        <v>0</v>
+      <c r="F199" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
@@ -5798,8 +5801,8 @@
       <c r="E200" s="2">
         <v>5690</v>
       </c>
-      <c r="F200" s="3">
-        <v>0</v>
+      <c r="F200" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
@@ -5858,8 +5861,8 @@
       <c r="E203" s="2">
         <v>7990</v>
       </c>
-      <c r="F203" s="3">
-        <v>0</v>
+      <c r="F203" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
@@ -5878,8 +5881,8 @@
       <c r="E204" s="2">
         <v>8990</v>
       </c>
-      <c r="F204" s="3">
-        <v>0</v>
+      <c r="F204" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
@@ -5898,8 +5901,8 @@
       <c r="E205" s="2">
         <v>10190</v>
       </c>
-      <c r="F205" s="3">
-        <v>0</v>
+      <c r="F205" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
@@ -5918,8 +5921,8 @@
       <c r="E206" s="2">
         <v>11690</v>
       </c>
-      <c r="F206" s="3">
-        <v>0</v>
+      <c r="F206" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
@@ -5938,8 +5941,8 @@
       <c r="E207" s="2">
         <v>7590</v>
       </c>
-      <c r="F207" s="3">
-        <v>0</v>
+      <c r="F207" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
@@ -5958,8 +5961,8 @@
       <c r="E208" s="2">
         <v>32990</v>
       </c>
-      <c r="F208" s="3">
-        <v>0</v>
+      <c r="F208" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
@@ -5978,8 +5981,8 @@
       <c r="E209" s="2">
         <v>6990</v>
       </c>
-      <c r="F209" s="3">
-        <v>0</v>
+      <c r="F209" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
@@ -5998,8 +6001,8 @@
       <c r="E210" s="2">
         <v>15990</v>
       </c>
-      <c r="F210" s="3">
-        <v>0</v>
+      <c r="F210" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
@@ -6034,8 +6037,8 @@
       <c r="E212" s="2">
         <v>700</v>
       </c>
-      <c r="F212" s="3">
-        <v>0</v>
+      <c r="F212" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
@@ -6074,8 +6077,8 @@
       <c r="E214" s="2">
         <v>13990</v>
       </c>
-      <c r="F214" s="3">
-        <v>0</v>
+      <c r="F214" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
@@ -6114,8 +6117,8 @@
       <c r="E216" s="2">
         <v>11990</v>
       </c>
-      <c r="F216" s="3">
-        <v>0</v>
+      <c r="F216" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
@@ -6134,8 +6137,8 @@
       <c r="E217" s="2">
         <v>12990</v>
       </c>
-      <c r="F217" s="3">
-        <v>0</v>
+      <c r="F217" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
@@ -6194,8 +6197,8 @@
       <c r="E220" s="2">
         <v>6190</v>
       </c>
-      <c r="F220" s="3">
-        <v>0</v>
+      <c r="F220" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
@@ -6214,8 +6217,8 @@
       <c r="E221" s="2">
         <v>6190</v>
       </c>
-      <c r="F221" s="3">
-        <v>0</v>
+      <c r="F221" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
@@ -6414,8 +6417,8 @@
       <c r="E231" s="2">
         <v>4290</v>
       </c>
-      <c r="F231" s="3">
-        <v>0</v>
+      <c r="F231" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
@@ -6434,8 +6437,8 @@
       <c r="E232" s="2">
         <v>4290</v>
       </c>
-      <c r="F232" s="3">
-        <v>0</v>
+      <c r="F232" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
@@ -6454,8 +6457,8 @@
       <c r="E233" s="2">
         <v>4290</v>
       </c>
-      <c r="F233" s="3">
-        <v>0</v>
+      <c r="F233" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
@@ -6474,8 +6477,8 @@
       <c r="E234" s="2">
         <v>2590</v>
       </c>
-      <c r="F234" s="3">
-        <v>0</v>
+      <c r="F234" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
@@ -7054,8 +7057,8 @@
       <c r="E263" s="2">
         <v>11990</v>
       </c>
-      <c r="F263" s="3">
-        <v>0</v>
+      <c r="F263" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
@@ -7074,8 +7077,8 @@
       <c r="E264" s="2">
         <v>11990</v>
       </c>
-      <c r="F264" s="3">
-        <v>0</v>
+      <c r="F264" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
@@ -7094,8 +7097,8 @@
       <c r="E265" s="2">
         <v>11990</v>
       </c>
-      <c r="F265" s="3">
-        <v>0</v>
+      <c r="F265" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
@@ -7114,8 +7117,8 @@
       <c r="E266" s="2">
         <v>11990</v>
       </c>
-      <c r="F266" s="3">
-        <v>0</v>
+      <c r="F266" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
@@ -7134,8 +7137,8 @@
       <c r="E267" s="2">
         <v>11990</v>
       </c>
-      <c r="F267" s="3">
-        <v>0</v>
+      <c r="F267" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
@@ -7154,8 +7157,8 @@
       <c r="E268" s="2">
         <v>11990</v>
       </c>
-      <c r="F268" s="3">
-        <v>0</v>
+      <c r="F268" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
@@ -7174,8 +7177,8 @@
       <c r="E269" s="2">
         <v>11990</v>
       </c>
-      <c r="F269" s="3">
-        <v>0</v>
+      <c r="F269" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
@@ -7214,8 +7217,8 @@
       <c r="E271" s="2">
         <v>3990</v>
       </c>
-      <c r="F271" s="3">
-        <v>0</v>
+      <c r="F271" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
@@ -7234,8 +7237,8 @@
       <c r="E272" s="2">
         <v>3990</v>
       </c>
-      <c r="F272" s="3">
-        <v>0</v>
+      <c r="F272" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
@@ -7254,8 +7257,8 @@
       <c r="E273" s="2">
         <v>4390</v>
       </c>
-      <c r="F273" s="3">
-        <v>0</v>
+      <c r="F273" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
@@ -7274,8 +7277,8 @@
       <c r="E274" s="2">
         <v>12990</v>
       </c>
-      <c r="F274" s="3">
-        <v>0</v>
+      <c r="F274" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
@@ -7294,8 +7297,8 @@
       <c r="E275" s="2">
         <v>4990</v>
       </c>
-      <c r="F275" s="3">
-        <v>0</v>
+      <c r="F275" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
@@ -7314,8 +7317,8 @@
       <c r="E276" s="2">
         <v>11990</v>
       </c>
-      <c r="F276" s="3">
-        <v>0</v>
+      <c r="F276" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
@@ -7334,8 +7337,8 @@
       <c r="E277" s="2">
         <v>4990</v>
       </c>
-      <c r="F277" s="3">
-        <v>0</v>
+      <c r="F277" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
@@ -7354,8 +7357,8 @@
       <c r="E278" s="2">
         <v>7990</v>
       </c>
-      <c r="F278" s="3">
-        <v>0</v>
+      <c r="F278" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.25">
@@ -7374,8 +7377,8 @@
       <c r="E279" s="2">
         <v>12490</v>
       </c>
-      <c r="F279" s="3">
-        <v>0</v>
+      <c r="F279" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
@@ -7394,8 +7397,8 @@
       <c r="E280" s="2">
         <v>4390</v>
       </c>
-      <c r="F280" s="3">
-        <v>0</v>
+      <c r="F280" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.25">
@@ -7414,8 +7417,8 @@
       <c r="E281" s="2">
         <v>4390</v>
       </c>
-      <c r="F281" s="3">
-        <v>0</v>
+      <c r="F281" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
@@ -7434,8 +7437,8 @@
       <c r="E282" s="2">
         <v>3990</v>
       </c>
-      <c r="F282" s="3">
-        <v>0</v>
+      <c r="F282" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
@@ -7454,8 +7457,8 @@
       <c r="E283" s="2">
         <v>11990</v>
       </c>
-      <c r="F283" s="3">
-        <v>0</v>
+      <c r="F283" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
@@ -7474,8 +7477,8 @@
       <c r="E284" s="2">
         <v>3990</v>
       </c>
-      <c r="F284" s="3">
-        <v>0</v>
+      <c r="F284" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.25">
@@ -7574,8 +7577,8 @@
       <c r="E289" s="2">
         <v>6990</v>
       </c>
-      <c r="F289" s="3">
-        <v>0</v>
+      <c r="F289" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
@@ -7594,8 +7597,8 @@
       <c r="E290" s="2">
         <v>8990</v>
       </c>
-      <c r="F290" s="3">
-        <v>0</v>
+      <c r="F290" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.25">
@@ -7614,8 +7617,8 @@
       <c r="E291" s="2">
         <v>6390</v>
       </c>
-      <c r="F291" s="3">
-        <v>0</v>
+      <c r="F291" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.25">
@@ -7634,8 +7637,8 @@
       <c r="E292" s="2">
         <v>22990</v>
       </c>
-      <c r="F292" s="3">
-        <v>0</v>
+      <c r="F292" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
@@ -7654,8 +7657,8 @@
       <c r="E293" s="2">
         <v>28990</v>
       </c>
-      <c r="F293" s="3">
-        <v>0</v>
+      <c r="F293" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.25">
@@ -7714,8 +7717,8 @@
       <c r="E296" s="2">
         <v>22990</v>
       </c>
-      <c r="F296" s="3">
-        <v>0</v>
+      <c r="F296" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.25">
@@ -7734,8 +7737,8 @@
       <c r="E297" s="2">
         <v>13990</v>
       </c>
-      <c r="F297" s="3">
-        <v>0</v>
+      <c r="F297" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.25">
@@ -7754,8 +7757,8 @@
       <c r="E298" s="2">
         <v>25990</v>
       </c>
-      <c r="F298" s="3">
-        <v>0</v>
+      <c r="F298" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.25">
@@ -7771,8 +7774,8 @@
       <c r="E299" s="2">
         <v>10</v>
       </c>
-      <c r="F299" s="3">
-        <v>0</v>
+      <c r="F299" t="s">
+        <v>466</v>
       </c>
     </row>
   </sheetData>

</xml_diff>